<commit_message>
add picCode for xh and hzg
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -2285,7 +2285,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2323,6 +2323,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2332,7 +2358,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2445,6 +2471,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5005,11 +5037,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K154"/>
+  <dimension ref="A1:K161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C160" sqref="C160"/>
+      <selection pane="bottomLeft" activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -6307,6 +6339,10 @@
       <c r="B154" s="3" t="s">
         <v>376</v>
       </c>
+    </row>
+    <row r="161" spans="2:3">
+      <c r="B161" s="38"/>
+      <c r="C161" s="39"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D153">
@@ -6331,7 +6367,7 @@
           <x14:formula1>
             <xm:f>status!$A$1:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C1048576</xm:sqref>
+          <xm:sqref>C1:C160 C162:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
forget commit little version
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -29,16 +29,15 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">input!$A$1:$D$27</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">proceding!$A$1:$K$180</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">proceding!$A$1:$K$194</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">小禾微贷!$A$5:$F$10</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="446">
   <si>
     <t>基本信息</t>
   </si>
@@ -2140,147 +2139,214 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>貌似解决了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>checkFilled after post successfully</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贷款超市 验证条件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贷款超市 头像上传</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lend_apply 页面 如果已成为贷款超市，显示list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>market list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据魔盒定时请求，查看是否完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>essential / optional config 合并，内部表示是否必填</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合并之后有问题啊。。。 首页无法获取啊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贷款超市 提交页面 滚动问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过贷款超市发起申请</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>option 组件用原生，样式重写</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>申请借款时 判断是贷款超市，显示贷款超市信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过marketId进入，显示贷款超市的信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>借贷宝，今借到，无忧借条，速速借及其它 放款平台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人分享放贷，提交参数 标识分享</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据魔盒的callback</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>session Storage 解决芝麻和数据魔盒的跳转问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>job_info 开放</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reapply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apply record</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0/1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>applyRecord.status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0/1/2/3/4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>占位符 路由，取代 query</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阻止贷款超市重复申请</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>负债调查 必填</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指定贷款超市的申请结果 和意见</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放贷超市 option 10px以下字体样式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apply borrow 里面加入是否有申请的判断</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个项目填写完成后，check了所有认证项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过申请记录 列表查看申请状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重构apply_borrow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>logo 加说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>logo上传 简化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贷款超市 | 个人信用评估   PS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贷款超市 申请放到 一级菜单</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>身份证上传简化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uniqueId 不展示手机号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>申请记录的金额显示问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简借的小禾</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>filter 全局化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>申请数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>申请条件+最低分数显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>申请后页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>微信分享 checkSession中配置无效，setInterval</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>貌似解决了</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>checkFilled after post successfully</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>贷款超市 验证条件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>贷款超市 头像上传</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lend_apply 页面 如果已成为贷款超市，显示list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>market list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据魔盒定时请求，查看是否完成</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>essential / optional config 合并，内部表示是否必填</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>合并之后有问题啊。。。 首页无法获取啊</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>贷款超市 提交页面 滚动问题</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>通过贷款超市发起申请</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>option 组件用原生，样式重写</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>申请借款时 判断是贷款超市，显示贷款超市信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>通过marketId进入，显示贷款超市的信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>借贷宝，今借到，无忧借条，速速借及其它 放款平台</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>个人分享放贷，提交参数 标识分享</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数据魔盒的callback</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>session Storage 解决芝麻和数据魔盒的跳转问题</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>job_info 开放</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reapply</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>apply record</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0/1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>applyRecord.status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0/1/2/3/4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>占位符 路由，取代 query</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>阻止贷款超市重复申请</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>负债调查 必填</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>指定贷款超市的申请结果 和意见</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>放贷超市 option 10px以下字体样式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>apply borrow 里面加入是否有申请的判断</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>每个项目填写完成后，check了所有认证项</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>贷款超市显示联系方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>申请加入金额</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晚上10.00到早上八点自动把更多借款的按钮放上</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2440,6 +2506,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -2582,7 +2656,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2723,6 +2797,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5374,7 +5451,7 @@
         <v>378</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F1" s="20" t="s">
         <v>379</v>
@@ -5437,7 +5514,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -5447,18 +5524,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B1" t="s">
         <v>416</v>
-      </c>
-      <c r="B1" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2" t="s">
         <v>418</v>
-      </c>
-      <c r="B2" t="s">
-        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -5470,11 +5547,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" filterMode="1"/>
-  <dimension ref="A1:K182"/>
+  <dimension ref="A1:K197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B187" sqref="B187"/>
+      <selection pane="bottomLeft" activeCell="D195" sqref="D195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -5482,8 +5559,8 @@
     <col min="1" max="1" width="9.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7265625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="5.1796875" style="39" customWidth="1"/>
-    <col min="5" max="5" width="3.81640625" style="39" customWidth="1"/>
+    <col min="4" max="4" width="8.26953125" style="39" customWidth="1"/>
+    <col min="5" max="5" width="4.26953125" style="39" customWidth="1"/>
     <col min="6" max="6" width="85" style="3" customWidth="1"/>
     <col min="7" max="7" width="84.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.26953125" bestFit="1" customWidth="1"/>
@@ -5500,10 +5577,10 @@
         <v>171</v>
       </c>
       <c r="D1" s="39" t="s">
+        <v>421</v>
+      </c>
+      <c r="E1" s="39" t="s">
         <v>422</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>423</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>172</v>
@@ -6821,9 +6898,12 @@
         <v>296</v>
       </c>
     </row>
-    <row r="127" spans="2:6">
+    <row r="127" spans="2:6" hidden="1">
       <c r="B127" s="3" t="s">
         <v>297</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="128" spans="2:6" hidden="1">
@@ -6849,9 +6929,12 @@
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" hidden="1">
       <c r="B130" s="3" t="s">
         <v>301</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="F130" s="3" t="s">
         <v>302</v>
@@ -6971,7 +7054,7 @@
         <v>327</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="144" spans="1:6" hidden="1">
@@ -7059,7 +7142,7 @@
     </row>
     <row r="152" spans="1:6">
       <c r="B152" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="153" spans="1:6">
@@ -7112,7 +7195,7 @@
     </row>
     <row r="159" spans="1:6">
       <c r="B159" s="3" t="s">
-        <v>395</v>
+        <v>442</v>
       </c>
       <c r="F159" s="3" t="s">
         <v>394</v>
@@ -7120,7 +7203,7 @@
     </row>
     <row r="160" spans="1:6" hidden="1">
       <c r="B160" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C160" s="3" t="s">
         <v>81</v>
@@ -7130,13 +7213,13 @@
     </row>
     <row r="161" spans="2:6">
       <c r="B161" s="33" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C161" s="34"/>
     </row>
     <row r="162" spans="2:6" hidden="1">
       <c r="B162" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C162" s="3" t="s">
         <v>193</v>
@@ -7146,7 +7229,7 @@
     </row>
     <row r="163" spans="2:6" hidden="1">
       <c r="B163" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C163" s="3" t="s">
         <v>81</v>
@@ -7156,7 +7239,7 @@
     </row>
     <row r="164" spans="2:6" hidden="1">
       <c r="B164" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>81</v>
@@ -7166,15 +7249,15 @@
     </row>
     <row r="165" spans="2:6">
       <c r="B165" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="F165" s="3" t="s">
         <v>403</v>
-      </c>
-      <c r="F165" s="3" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="166" spans="2:6" hidden="1">
       <c r="B166" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C166" s="3" t="s">
         <v>81</v>
@@ -7184,7 +7267,7 @@
     </row>
     <row r="167" spans="2:6" hidden="1">
       <c r="B167" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C167" s="3" t="s">
         <v>81</v>
@@ -7194,7 +7277,7 @@
     </row>
     <row r="168" spans="2:6" hidden="1">
       <c r="B168" s="7" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C168" s="3" t="s">
         <v>81</v>
@@ -7204,7 +7287,7 @@
     </row>
     <row r="169" spans="2:6" hidden="1">
       <c r="B169" s="35" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C169" s="3" t="s">
         <v>81</v>
@@ -7212,17 +7295,17 @@
       <c r="D169" s="3"/>
       <c r="E169" s="3"/>
       <c r="F169" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="170" spans="2:6">
       <c r="B170" s="7" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="171" spans="2:6" hidden="1">
       <c r="B171" s="35" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C171" s="3" t="s">
         <v>81</v>
@@ -7236,7 +7319,7 @@
     </row>
     <row r="172" spans="2:6" hidden="1">
       <c r="B172" s="7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C172" s="3" t="s">
         <v>81</v>
@@ -7244,20 +7327,23 @@
       <c r="D172" s="3"/>
       <c r="E172" s="3"/>
     </row>
-    <row r="173" spans="2:6">
+    <row r="173" spans="2:6" hidden="1">
       <c r="B173" s="7" t="s">
-        <v>411</v>
+        <v>410</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="D173" s="40"/>
     </row>
     <row r="174" spans="2:6">
       <c r="B174" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="175" spans="2:6">
       <c r="B175" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C175" s="3" t="s">
         <v>118</v>
@@ -7265,15 +7351,15 @@
     </row>
     <row r="176" spans="2:6">
       <c r="B176" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="177" spans="2:6" hidden="1">
+    <row r="177" spans="1:6" hidden="1">
       <c r="B177" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C177" s="3" t="s">
         <v>81</v>
@@ -7281,14 +7367,14 @@
       <c r="D177" s="3"/>
       <c r="E177" s="3"/>
     </row>
-    <row r="178" spans="2:6">
-      <c r="B178" s="3" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="179" spans="2:6" hidden="1">
+    <row r="178" spans="1:6">
+      <c r="B178" s="47" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" hidden="1">
       <c r="B179" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C179" s="3" t="s">
         <v>81</v>
@@ -7300,9 +7386,9 @@
         <v>0.68888888888888899</v>
       </c>
     </row>
-    <row r="180" spans="2:6" hidden="1">
+    <row r="180" spans="1:6" hidden="1">
       <c r="B180" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C180" s="3" t="s">
         <v>81</v>
@@ -7315,15 +7401,173 @@
       </c>
       <c r="F180" s="36"/>
     </row>
-    <row r="182" spans="2:6">
+    <row r="181" spans="1:6">
+      <c r="B181" s="7" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
       <c r="B182" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
+      <c r="B183" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" hidden="1">
+      <c r="B184" s="35" t="s">
+        <v>433</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" hidden="1">
+      <c r="B185" s="35" t="s">
+        <v>430</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F185" s="3" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" hidden="1">
+      <c r="B186" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D186" s="40">
+        <v>42959</v>
+      </c>
+      <c r="E186" s="41">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" hidden="1">
+      <c r="B187" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D187" s="40">
+        <v>42960</v>
+      </c>
+      <c r="E187" s="41">
+        <v>8.8888888888888892E-2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" hidden="1">
+      <c r="B188" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D188" s="40">
+        <v>42960</v>
+      </c>
+      <c r="E188" s="41">
+        <v>8.8888888888888892E-2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" hidden="1">
+      <c r="A189" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D189" s="40">
+        <v>42960</v>
+      </c>
+      <c r="E189" s="41">
+        <v>0.10972222222222222</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" hidden="1">
+      <c r="B190" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D190" s="40">
+        <v>42960</v>
+      </c>
+      <c r="E190" s="41">
+        <v>0.52638888888888891</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6">
+      <c r="B191" s="3" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6">
+      <c r="B192" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="D192" s="40">
+        <v>42961</v>
+      </c>
+      <c r="E192" s="41">
+        <v>0.9868055555555556</v>
+      </c>
+    </row>
+    <row r="193" spans="2:5" hidden="1">
+      <c r="B193" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D193" s="40">
+        <v>42961</v>
+      </c>
+      <c r="E193" s="41">
+        <v>0.9868055555555556</v>
+      </c>
+    </row>
+    <row r="194" spans="2:5">
+      <c r="B194" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="D194" s="40">
+        <v>42962</v>
+      </c>
+      <c r="E194" s="41">
+        <v>2.8472222222222222E-2</v>
+      </c>
+    </row>
+    <row r="195" spans="2:5">
+      <c r="B195" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="196" spans="2:5">
+      <c r="B196" s="3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="197" spans="2:5">
+      <c r="B197" s="3" t="s">
+        <v>445</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K180">
+  <autoFilter ref="A1:K194">
     <filterColumn colId="2">
-      <filters>
+      <filters blank="1">
         <filter val="pendding"/>
       </filters>
     </filterColumn>
@@ -7342,7 +7586,7 @@
           <x14:formula1>
             <xm:f>status!$A$1:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C162:C1048576 C1:C160</xm:sqref>
+          <xm:sqref>C1:C160 C162:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
hzg changing market list css
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -2340,6 +2340,7 @@
   </si>
   <si>
     <t>晚上10.00到早上八点自动把更多借款的按钮放上</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2783,6 +2784,9 @@
     <xf numFmtId="20" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2797,9 +2801,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4882,12 +4883,12 @@
       </c>
     </row>
     <row r="24" spans="25:30">
-      <c r="AA24" s="46" t="s">
+      <c r="AA24" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="AB24" s="46"/>
-      <c r="AC24" s="46"/>
-      <c r="AD24" s="46"/>
+      <c r="AB24" s="47"/>
+      <c r="AC24" s="47"/>
+      <c r="AD24" s="47"/>
     </row>
     <row r="28" spans="25:30">
       <c r="Z28" s="28" t="s">
@@ -4903,43 +4904,43 @@
       </c>
     </row>
     <row r="37" spans="1:30">
-      <c r="A37" s="45" t="s">
+      <c r="A37" s="46" t="s">
         <v>338</v>
       </c>
-      <c r="B37" s="45"/>
+      <c r="B37" s="46"/>
     </row>
     <row r="38" spans="1:30">
-      <c r="A38" s="45"/>
-      <c r="B38" s="45"/>
+      <c r="A38" s="46"/>
+      <c r="B38" s="46"/>
     </row>
     <row r="39" spans="1:30">
-      <c r="A39" s="45"/>
-      <c r="B39" s="45"/>
+      <c r="A39" s="46"/>
+      <c r="B39" s="46"/>
     </row>
     <row r="40" spans="1:30">
-      <c r="A40" s="45"/>
-      <c r="B40" s="45"/>
+      <c r="A40" s="46"/>
+      <c r="B40" s="46"/>
       <c r="S40" s="27" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="41" spans="1:30">
-      <c r="A41" s="45"/>
-      <c r="B41" s="45"/>
+      <c r="A41" s="46"/>
+      <c r="B41" s="46"/>
       <c r="R41" s="27" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="42" spans="1:30">
-      <c r="A42" s="45"/>
-      <c r="B42" s="45"/>
+      <c r="A42" s="46"/>
+      <c r="B42" s="46"/>
       <c r="Q42" s="27" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="43" spans="1:30">
-      <c r="A43" s="45"/>
-      <c r="B43" s="45"/>
+      <c r="A43" s="46"/>
+      <c r="B43" s="46"/>
       <c r="G43" s="27" t="s">
         <v>342</v>
       </c>
@@ -4951,8 +4952,8 @@
       </c>
     </row>
     <row r="44" spans="1:30">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
+      <c r="A44" s="46"/>
+      <c r="B44" s="46"/>
       <c r="G44" s="27" t="s">
         <v>341</v>
       </c>
@@ -4965,16 +4966,16 @@
       <c r="O44" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="AA44" s="46" t="s">
+      <c r="AA44" s="47" t="s">
         <v>353</v>
       </c>
-      <c r="AB44" s="46"/>
-      <c r="AC44" s="46"/>
-      <c r="AD44" s="46"/>
+      <c r="AB44" s="47"/>
+      <c r="AC44" s="47"/>
+      <c r="AD44" s="47"/>
     </row>
     <row r="45" spans="1:30">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
+      <c r="A45" s="46"/>
+      <c r="B45" s="46"/>
       <c r="K45" s="29" t="s">
         <v>340</v>
       </c>
@@ -4987,8 +4988,8 @@
       </c>
     </row>
     <row r="46" spans="1:30">
-      <c r="A46" s="45"/>
-      <c r="B46" s="45"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
       <c r="K46" s="29" t="s">
         <v>340</v>
       </c>
@@ -5001,8 +5002,8 @@
       </c>
     </row>
     <row r="47" spans="1:30">
-      <c r="A47" s="45"/>
-      <c r="B47" s="45"/>
+      <c r="A47" s="46"/>
+      <c r="B47" s="46"/>
       <c r="K47" s="29" t="s">
         <v>340</v>
       </c>
@@ -5015,8 +5016,8 @@
       </c>
     </row>
     <row r="48" spans="1:30">
-      <c r="A48" s="45"/>
-      <c r="B48" s="45"/>
+      <c r="A48" s="46"/>
+      <c r="B48" s="46"/>
       <c r="K48" s="29" t="s">
         <v>340</v>
       </c>
@@ -5029,8 +5030,8 @@
       </c>
     </row>
     <row r="49" spans="1:26">
-      <c r="A49" s="45"/>
-      <c r="B49" s="45"/>
+      <c r="A49" s="46"/>
+      <c r="B49" s="46"/>
       <c r="K49" s="29" t="s">
         <v>340</v>
       </c>
@@ -5046,8 +5047,8 @@
       </c>
     </row>
     <row r="50" spans="1:26">
-      <c r="A50" s="45"/>
-      <c r="B50" s="45"/>
+      <c r="A50" s="46"/>
+      <c r="B50" s="46"/>
       <c r="K50" s="29" t="s">
         <v>340</v>
       </c>
@@ -5063,8 +5064,8 @@
       </c>
     </row>
     <row r="51" spans="1:26">
-      <c r="A51" s="45"/>
-      <c r="B51" s="45"/>
+      <c r="A51" s="46"/>
+      <c r="B51" s="46"/>
       <c r="K51" s="29" t="s">
         <v>340</v>
       </c>
@@ -5074,8 +5075,8 @@
       </c>
     </row>
     <row r="52" spans="1:26">
-      <c r="A52" s="45"/>
-      <c r="B52" s="45"/>
+      <c r="A52" s="46"/>
+      <c r="B52" s="46"/>
       <c r="K52" s="29" t="s">
         <v>340</v>
       </c>
@@ -5144,59 +5145,59 @@
       </c>
     </row>
     <row r="60" spans="1:26">
-      <c r="A60" s="45" t="s">
+      <c r="A60" s="46" t="s">
         <v>339</v>
       </c>
-      <c r="B60" s="45"/>
+      <c r="B60" s="46"/>
       <c r="N60" s="29" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="61" spans="1:26">
-      <c r="A61" s="45"/>
-      <c r="B61" s="45"/>
+      <c r="A61" s="46"/>
+      <c r="B61" s="46"/>
       <c r="N61" s="29" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="62" spans="1:26">
-      <c r="A62" s="45"/>
-      <c r="B62" s="45"/>
+      <c r="A62" s="46"/>
+      <c r="B62" s="46"/>
       <c r="N62" s="29" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="63" spans="1:26">
-      <c r="A63" s="45"/>
-      <c r="B63" s="45"/>
+      <c r="A63" s="46"/>
+      <c r="B63" s="46"/>
       <c r="N63" s="29" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="64" spans="1:26">
-      <c r="A64" s="45"/>
-      <c r="B64" s="45"/>
+      <c r="A64" s="46"/>
+      <c r="B64" s="46"/>
       <c r="N64" s="29" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="65" spans="1:21">
-      <c r="A65" s="45"/>
-      <c r="B65" s="45"/>
+      <c r="A65" s="46"/>
+      <c r="B65" s="46"/>
       <c r="N65" s="29" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="66" spans="1:21">
-      <c r="A66" s="45"/>
-      <c r="B66" s="45"/>
+      <c r="A66" s="46"/>
+      <c r="B66" s="46"/>
       <c r="N66" s="29" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="67" spans="1:21">
-      <c r="A67" s="45"/>
-      <c r="B67" s="45"/>
+      <c r="A67" s="46"/>
+      <c r="B67" s="46"/>
       <c r="M67" s="27" t="s">
         <v>341</v>
       </c>
@@ -5226,28 +5227,28 @@
       </c>
     </row>
     <row r="68" spans="1:21">
-      <c r="A68" s="45"/>
-      <c r="B68" s="45"/>
+      <c r="A68" s="46"/>
+      <c r="B68" s="46"/>
     </row>
     <row r="69" spans="1:21">
-      <c r="A69" s="45"/>
-      <c r="B69" s="45"/>
+      <c r="A69" s="46"/>
+      <c r="B69" s="46"/>
     </row>
     <row r="70" spans="1:21">
-      <c r="A70" s="45"/>
-      <c r="B70" s="45"/>
+      <c r="A70" s="46"/>
+      <c r="B70" s="46"/>
     </row>
     <row r="71" spans="1:21">
-      <c r="A71" s="45"/>
-      <c r="B71" s="45"/>
+      <c r="A71" s="46"/>
+      <c r="B71" s="46"/>
     </row>
     <row r="72" spans="1:21">
-      <c r="A72" s="45"/>
-      <c r="B72" s="45"/>
+      <c r="A72" s="46"/>
+      <c r="B72" s="46"/>
     </row>
     <row r="73" spans="1:21">
-      <c r="A73" s="45"/>
-      <c r="B73" s="45"/>
+      <c r="A73" s="46"/>
+      <c r="B73" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5550,8 +5551,8 @@
   <dimension ref="A1:K197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D195" sqref="D195"/>
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B199" sqref="B199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -7368,7 +7369,7 @@
       <c r="E177" s="3"/>
     </row>
     <row r="178" spans="1:6">
-      <c r="B178" s="47" t="s">
+      <c r="B178" s="42" t="s">
         <v>426</v>
       </c>
     </row>
@@ -7567,7 +7568,7 @@
   </sheetData>
   <autoFilter ref="A1:K194">
     <filterColumn colId="2">
-      <filters blank="1">
+      <filters>
         <filter val="pendding"/>
       </filters>
     </filterColumn>
@@ -7700,27 +7701,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
     </row>
     <row r="2" spans="2:8">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="F2" s="42" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="F2" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="12" spans="2:8">
       <c r="E12" t="s">
@@ -7751,36 +7752,36 @@
   <sheetFormatPr defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="2:12">
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
     </row>
     <row r="2" spans="2:12">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="F2" s="42" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="F2" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="J2" s="42" t="s">
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="J2" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
     </row>
     <row r="10" spans="2:12">
       <c r="E10" t="s">

</xml_diff>

<commit_message>
amend a bug markek_list goP function
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="444">
   <si>
     <t>基本信息</t>
   </si>
@@ -2331,15 +2331,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>贷款超市显示联系方式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>申请加入金额</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>晚上10.00到早上八点自动把更多借款的按钮放上</t>
+    <t>小禾 禾掌柜 拆fen不同的repository</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2783,6 +2776,9 @@
     <xf numFmtId="20" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2797,9 +2793,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4882,12 +4875,12 @@
       </c>
     </row>
     <row r="24" spans="25:30">
-      <c r="AA24" s="46" t="s">
+      <c r="AA24" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="AB24" s="46"/>
-      <c r="AC24" s="46"/>
-      <c r="AD24" s="46"/>
+      <c r="AB24" s="47"/>
+      <c r="AC24" s="47"/>
+      <c r="AD24" s="47"/>
     </row>
     <row r="28" spans="25:30">
       <c r="Z28" s="28" t="s">
@@ -4903,43 +4896,43 @@
       </c>
     </row>
     <row r="37" spans="1:30">
-      <c r="A37" s="45" t="s">
+      <c r="A37" s="46" t="s">
         <v>338</v>
       </c>
-      <c r="B37" s="45"/>
+      <c r="B37" s="46"/>
     </row>
     <row r="38" spans="1:30">
-      <c r="A38" s="45"/>
-      <c r="B38" s="45"/>
+      <c r="A38" s="46"/>
+      <c r="B38" s="46"/>
     </row>
     <row r="39" spans="1:30">
-      <c r="A39" s="45"/>
-      <c r="B39" s="45"/>
+      <c r="A39" s="46"/>
+      <c r="B39" s="46"/>
     </row>
     <row r="40" spans="1:30">
-      <c r="A40" s="45"/>
-      <c r="B40" s="45"/>
+      <c r="A40" s="46"/>
+      <c r="B40" s="46"/>
       <c r="S40" s="27" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="41" spans="1:30">
-      <c r="A41" s="45"/>
-      <c r="B41" s="45"/>
+      <c r="A41" s="46"/>
+      <c r="B41" s="46"/>
       <c r="R41" s="27" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="42" spans="1:30">
-      <c r="A42" s="45"/>
-      <c r="B42" s="45"/>
+      <c r="A42" s="46"/>
+      <c r="B42" s="46"/>
       <c r="Q42" s="27" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="43" spans="1:30">
-      <c r="A43" s="45"/>
-      <c r="B43" s="45"/>
+      <c r="A43" s="46"/>
+      <c r="B43" s="46"/>
       <c r="G43" s="27" t="s">
         <v>342</v>
       </c>
@@ -4951,8 +4944,8 @@
       </c>
     </row>
     <row r="44" spans="1:30">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
+      <c r="A44" s="46"/>
+      <c r="B44" s="46"/>
       <c r="G44" s="27" t="s">
         <v>341</v>
       </c>
@@ -4965,16 +4958,16 @@
       <c r="O44" s="27" t="s">
         <v>347</v>
       </c>
-      <c r="AA44" s="46" t="s">
+      <c r="AA44" s="47" t="s">
         <v>353</v>
       </c>
-      <c r="AB44" s="46"/>
-      <c r="AC44" s="46"/>
-      <c r="AD44" s="46"/>
+      <c r="AB44" s="47"/>
+      <c r="AC44" s="47"/>
+      <c r="AD44" s="47"/>
     </row>
     <row r="45" spans="1:30">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
+      <c r="A45" s="46"/>
+      <c r="B45" s="46"/>
       <c r="K45" s="29" t="s">
         <v>340</v>
       </c>
@@ -4987,8 +4980,8 @@
       </c>
     </row>
     <row r="46" spans="1:30">
-      <c r="A46" s="45"/>
-      <c r="B46" s="45"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
       <c r="K46" s="29" t="s">
         <v>340</v>
       </c>
@@ -5001,8 +4994,8 @@
       </c>
     </row>
     <row r="47" spans="1:30">
-      <c r="A47" s="45"/>
-      <c r="B47" s="45"/>
+      <c r="A47" s="46"/>
+      <c r="B47" s="46"/>
       <c r="K47" s="29" t="s">
         <v>340</v>
       </c>
@@ -5015,8 +5008,8 @@
       </c>
     </row>
     <row r="48" spans="1:30">
-      <c r="A48" s="45"/>
-      <c r="B48" s="45"/>
+      <c r="A48" s="46"/>
+      <c r="B48" s="46"/>
       <c r="K48" s="29" t="s">
         <v>340</v>
       </c>
@@ -5029,8 +5022,8 @@
       </c>
     </row>
     <row r="49" spans="1:26">
-      <c r="A49" s="45"/>
-      <c r="B49" s="45"/>
+      <c r="A49" s="46"/>
+      <c r="B49" s="46"/>
       <c r="K49" s="29" t="s">
         <v>340</v>
       </c>
@@ -5046,8 +5039,8 @@
       </c>
     </row>
     <row r="50" spans="1:26">
-      <c r="A50" s="45"/>
-      <c r="B50" s="45"/>
+      <c r="A50" s="46"/>
+      <c r="B50" s="46"/>
       <c r="K50" s="29" t="s">
         <v>340</v>
       </c>
@@ -5063,8 +5056,8 @@
       </c>
     </row>
     <row r="51" spans="1:26">
-      <c r="A51" s="45"/>
-      <c r="B51" s="45"/>
+      <c r="A51" s="46"/>
+      <c r="B51" s="46"/>
       <c r="K51" s="29" t="s">
         <v>340</v>
       </c>
@@ -5074,8 +5067,8 @@
       </c>
     </row>
     <row r="52" spans="1:26">
-      <c r="A52" s="45"/>
-      <c r="B52" s="45"/>
+      <c r="A52" s="46"/>
+      <c r="B52" s="46"/>
       <c r="K52" s="29" t="s">
         <v>340</v>
       </c>
@@ -5144,59 +5137,59 @@
       </c>
     </row>
     <row r="60" spans="1:26">
-      <c r="A60" s="45" t="s">
+      <c r="A60" s="46" t="s">
         <v>339</v>
       </c>
-      <c r="B60" s="45"/>
+      <c r="B60" s="46"/>
       <c r="N60" s="29" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="61" spans="1:26">
-      <c r="A61" s="45"/>
-      <c r="B61" s="45"/>
+      <c r="A61" s="46"/>
+      <c r="B61" s="46"/>
       <c r="N61" s="29" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="62" spans="1:26">
-      <c r="A62" s="45"/>
-      <c r="B62" s="45"/>
+      <c r="A62" s="46"/>
+      <c r="B62" s="46"/>
       <c r="N62" s="29" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="63" spans="1:26">
-      <c r="A63" s="45"/>
-      <c r="B63" s="45"/>
+      <c r="A63" s="46"/>
+      <c r="B63" s="46"/>
       <c r="N63" s="29" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="64" spans="1:26">
-      <c r="A64" s="45"/>
-      <c r="B64" s="45"/>
+      <c r="A64" s="46"/>
+      <c r="B64" s="46"/>
       <c r="N64" s="29" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="65" spans="1:21">
-      <c r="A65" s="45"/>
-      <c r="B65" s="45"/>
+      <c r="A65" s="46"/>
+      <c r="B65" s="46"/>
       <c r="N65" s="29" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="66" spans="1:21">
-      <c r="A66" s="45"/>
-      <c r="B66" s="45"/>
+      <c r="A66" s="46"/>
+      <c r="B66" s="46"/>
       <c r="N66" s="29" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="67" spans="1:21">
-      <c r="A67" s="45"/>
-      <c r="B67" s="45"/>
+      <c r="A67" s="46"/>
+      <c r="B67" s="46"/>
       <c r="M67" s="27" t="s">
         <v>341</v>
       </c>
@@ -5226,28 +5219,28 @@
       </c>
     </row>
     <row r="68" spans="1:21">
-      <c r="A68" s="45"/>
-      <c r="B68" s="45"/>
+      <c r="A68" s="46"/>
+      <c r="B68" s="46"/>
     </row>
     <row r="69" spans="1:21">
-      <c r="A69" s="45"/>
-      <c r="B69" s="45"/>
+      <c r="A69" s="46"/>
+      <c r="B69" s="46"/>
     </row>
     <row r="70" spans="1:21">
-      <c r="A70" s="45"/>
-      <c r="B70" s="45"/>
+      <c r="A70" s="46"/>
+      <c r="B70" s="46"/>
     </row>
     <row r="71" spans="1:21">
-      <c r="A71" s="45"/>
-      <c r="B71" s="45"/>
+      <c r="A71" s="46"/>
+      <c r="B71" s="46"/>
     </row>
     <row r="72" spans="1:21">
-      <c r="A72" s="45"/>
-      <c r="B72" s="45"/>
+      <c r="A72" s="46"/>
+      <c r="B72" s="46"/>
     </row>
     <row r="73" spans="1:21">
-      <c r="A73" s="45"/>
-      <c r="B73" s="45"/>
+      <c r="A73" s="46"/>
+      <c r="B73" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5547,11 +5540,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" filterMode="1"/>
-  <dimension ref="A1:K197"/>
+  <dimension ref="A1:K196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D195" sqref="D195"/>
+      <pane ySplit="1" topLeftCell="A195" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B202" sqref="B202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -7368,7 +7361,7 @@
       <c r="E177" s="3"/>
     </row>
     <row r="178" spans="1:6">
-      <c r="B178" s="47" t="s">
+      <c r="B178" s="42" t="s">
         <v>426</v>
       </c>
     </row>
@@ -7549,25 +7542,15 @@
         <v>2.8472222222222222E-2</v>
       </c>
     </row>
-    <row r="195" spans="2:5">
-      <c r="B195" s="3" t="s">
-        <v>443</v>
-      </c>
-    </row>
     <row r="196" spans="2:5">
       <c r="B196" s="3" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="197" spans="2:5">
-      <c r="B197" s="3" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K194">
     <filterColumn colId="2">
-      <filters blank="1">
+      <filters>
         <filter val="pendding"/>
       </filters>
     </filterColumn>
@@ -7700,27 +7683,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
     </row>
     <row r="2" spans="2:8">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="F2" s="42" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="F2" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="12" spans="2:8">
       <c r="E12" t="s">
@@ -7751,36 +7734,36 @@
   <sheetFormatPr defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="2:12">
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
     </row>
     <row r="2" spans="2:12">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="F2" s="42" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="F2" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="J2" s="42" t="s">
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="J2" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
     </row>
     <row r="10" spans="2:12">
       <c r="E10" t="s">

</xml_diff>